<commit_message>
On branch main # Changes to be committed: #	modified:   FTZ_APP/logs/ftz_app_usage_log.xlsx
</commit_message>
<xml_diff>
--- a/FTZ_APP/logs/ftz_app_usage_log.xlsx
+++ b/FTZ_APP/logs/ftz_app_usage_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>timestamp</t>
   </si>
@@ -76,6 +76,9 @@
     <t>2026-01-08 22:05:28 EST</t>
   </si>
   <si>
+    <t>2026-01-08 23:21:28 EST</t>
+  </si>
+  <si>
     <t>eb968125-9a60-4092-a9e3-7208dd222f84</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>9a701582-dd83-4f71-b143-a5b6e0823fba</t>
+  </si>
+  <si>
+    <t>c1b327ad-ea0c-473d-89e7-ac6a496a5767</t>
   </si>
   <si>
     <t>No</t>
@@ -473,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,7 +528,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>-215000</v>
@@ -534,7 +540,7 @@
         <v>1591330</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -542,7 +548,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>-215000</v>
@@ -554,19 +560,19 @@
         <v>1591330</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -574,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>-215000</v>
@@ -586,10 +592,10 @@
         <v>1591330</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,7 +603,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>-215000</v>
@@ -609,7 +615,7 @@
         <v>1591330</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -617,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>-215000</v>
@@ -629,7 +635,7 @@
         <v>1591330</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -637,7 +643,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>-215000</v>
@@ -649,10 +655,10 @@
         <v>1591330</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -660,7 +666,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>-215000</v>
@@ -672,19 +678,19 @@
         <v>1591330</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -692,7 +698,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>-215000</v>
@@ -704,7 +710,27 @@
         <v>1591330</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>-215000</v>
+      </c>
+      <c r="D10">
+        <v>1806330</v>
+      </c>
+      <c r="E10">
+        <v>1591330</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>